<commit_message>
T3 avanzado, y punto a FCFS corregido
</commit_message>
<xml_diff>
--- a/Clases Jueves/Actividad 1/punto a FCFS.xlsx
+++ b/Clases Jueves/Actividad 1/punto a FCFS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UADER\Tercero\Sistemas operativos\Actividad 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Desktop\tercero\Sistemas Operativos\Sistemas-Operativos\Clases Jueves\Actividad 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{176E8774-BD4F-426C-9344-9FB5037D4F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1F4AF2-2F01-46F0-89E4-A36F36434FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8490" yWindow="4245" windowWidth="22365" windowHeight="8880" xr2:uid="{6A0ACBF7-84F8-4B0F-82CC-BC039943834F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" xr2:uid="{6A0ACBF7-84F8-4B0F-82CC-BC039943834F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -76,13 +76,19 @@
   </si>
   <si>
     <t>T. Espera</t>
+  </si>
+  <si>
+    <t>ESPERA</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,8 +111,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,8 +152,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -168,50 +195,154 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -219,11 +350,83 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,87 +743,139 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A158255-1952-4FBD-B22B-CE483D220399}">
   <dimension ref="A4:AM19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
-    <col min="2" max="39" width="3.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="39" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="S4" s="9" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="V4" s="9"/>
-      <c r="W4" s="5" t="s">
+      <c r="I4" s="19"/>
+      <c r="J4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="19"/>
+      <c r="M4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="X4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y4" s="9"/>
-    </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="N4" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="38"/>
+      <c r="P4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="4" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="4" t="s">
+      <c r="H5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="M5" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="25"/>
+      <c r="O5" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="B6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="K6" s="35"/>
+      <c r="L6" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="28"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
@@ -738,51 +993,51 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="12"/>
-      <c r="AA8" s="12"/>
-      <c r="AB8" s="12"/>
-      <c r="AC8" s="12"/>
-      <c r="AD8" s="12"/>
-      <c r="AE8" s="12"/>
-      <c r="AF8" s="12"/>
-      <c r="AG8" s="12"/>
-      <c r="AH8" s="12"/>
-      <c r="AI8" s="12"/>
-      <c r="AJ8" s="12"/>
-      <c r="AK8" s="12"/>
-      <c r="AL8" s="12"/>
-      <c r="AM8" s="12"/>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="10"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
       <c r="B9" s="1">
         <v>0</v>
       </c>
@@ -898,196 +1153,202 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18" t="s">
+      <c r="G11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="J11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="20" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="19" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="13"/>
+      <c r="I12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="J12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="14">
         <v>8</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2">
-        <f>8 + 0</f>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14">
+        <v>5</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14">
+        <v>13</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="14">
         <v>8</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14">
+        <v>5</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14">
+        <f>8 + 5</f>
+        <v>13</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="14">
         <v>8</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2">
-        <v>7</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2">
-        <f>8+7</f>
-        <v>15</v>
-      </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2">
-        <v>8</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2">
-        <f>6+7</f>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14">
+        <v>6</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14">
+        <f>8+5</f>
         <v>13</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2">
-        <f>6+7+8</f>
-        <v>21</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="L17" s="39"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
         <f>SUM(H15:H17)/3</f>
-        <v>14.666666666666666</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2">
+        <v>13</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14">
         <f>SUM(E15:E17)/3</f>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="A18:C18"/>
+  <mergeCells count="41">
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="D18:G18"/>
     <mergeCell ref="D19:G19"/>
@@ -1101,8 +1362,7 @@
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="B17:D17"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="S4:T4"/>
     <mergeCell ref="U4:V4"/>
     <mergeCell ref="X4:Y4"/>
@@ -1114,13 +1374,14 @@
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="J12:K12"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
     <mergeCell ref="B8:AM8"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="E6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>